<commit_message>
fix wrong format money in sample data file
</commit_message>
<xml_diff>
--- a/data.xlsx
+++ b/data.xlsx
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="64" uniqueCount="55">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="69" uniqueCount="60">
   <si>
     <t>Id</t>
   </si>
@@ -186,6 +186,21 @@
   </si>
   <si>
     <t>2,04</t>
+  </si>
+  <si>
+    <t>200.400</t>
+  </si>
+  <si>
+    <t>199.000</t>
+  </si>
+  <si>
+    <t>300.000</t>
+  </si>
+  <si>
+    <t>105.000</t>
+  </si>
+  <si>
+    <t>204.000</t>
   </si>
 </sst>
 </file>
@@ -259,7 +274,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
@@ -283,6 +298,9 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="9" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -568,7 +586,7 @@
   <dimension ref="A1:G6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F18" sqref="F18"/>
+      <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -955,7 +973,7 @@
   <dimension ref="A1:E24"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="S7" sqref="S7"/>
+      <selection activeCell="O12" sqref="O12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1112,8 +1130,8 @@
       <c r="C9" s="4">
         <v>2</v>
       </c>
-      <c r="D9" s="4">
-        <v>200.4</v>
+      <c r="D9" s="9" t="s">
+        <v>55</v>
       </c>
       <c r="E9" s="6">
         <v>43817</v>
@@ -1163,8 +1181,8 @@
       <c r="C12" s="4" t="s">
         <v>48</v>
       </c>
-      <c r="D12" s="4">
-        <v>199</v>
+      <c r="D12" s="9" t="s">
+        <v>56</v>
       </c>
       <c r="E12" s="6">
         <v>43817</v>
@@ -1214,8 +1232,8 @@
       <c r="C15" s="4">
         <v>3</v>
       </c>
-      <c r="D15" s="4">
-        <v>300</v>
+      <c r="D15" s="9" t="s">
+        <v>57</v>
       </c>
       <c r="E15" s="6">
         <v>43817</v>
@@ -1265,8 +1283,8 @@
       <c r="C18" s="4" t="s">
         <v>52</v>
       </c>
-      <c r="D18" s="4">
-        <v>105</v>
+      <c r="D18" s="9" t="s">
+        <v>58</v>
       </c>
       <c r="E18" s="6">
         <v>43818</v>
@@ -1316,8 +1334,8 @@
       <c r="C21" s="4" t="s">
         <v>54</v>
       </c>
-      <c r="D21" s="4">
-        <v>204</v>
+      <c r="D21" s="9" t="s">
+        <v>59</v>
       </c>
       <c r="E21" s="6">
         <v>43817</v>

</xml_diff>